<commit_message>
fix item excel form
</commit_message>
<xml_diff>
--- a/application/controllers/Items.xlsx
+++ b/application/controllers/Items.xlsx
@@ -67,11 +67,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="333375" cy="333375"/>
+    <xdr:ext cx="714375" cy="714375"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Sample image" descr="Sample image"/>
@@ -387,7 +387,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -395,8 +395,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="2" spans="1:1">
-      <c r="A2"/>
+    <row r="1" spans="1:1">
+      <c r="A1"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>